<commit_message>
[feature] add validation for file excel
</commit_message>
<xml_diff>
--- a/src/main/resources/fileTemplate/Financial Planning_v1.0.xlsx
+++ b/src/main/resources/fileTemplate/Financial Planning_v1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\IdeaProjects\fin-planning-backend\src\main\resources\fileTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA763ED2-5C20-4156-AB2E-A95D90D8599F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A480880E-62F5-4C8F-8ED9-A8CC252A20C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2064" yWindow="720" windowWidth="20520" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expense" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>DATE</t>
   </si>
@@ -41,12 +41,6 @@
   </si>
   <si>
     <t>ID</t>
-  </si>
-  <si>
-    <t>HR</t>
-  </si>
-  <si>
-    <t>Marketing</t>
   </si>
   <si>
     <t>Department</t>
@@ -103,36 +97,6 @@
     <t>STATUS</t>
   </si>
   <si>
-    <t>Indirect Costs.</t>
-  </si>
-  <si>
-    <t>Administration Costs.</t>
-  </si>
-  <si>
-    <t>Operating Costs.</t>
-  </si>
-  <si>
-    <t>Maintenance Costs.</t>
-  </si>
-  <si>
-    <t>Manufacturing costs</t>
-  </si>
-  <si>
-    <t>Direct Costs.</t>
-  </si>
-  <si>
-    <t>IT</t>
-  </si>
-  <si>
-    <t>Finance</t>
-  </si>
-  <si>
-    <t>Communication</t>
-  </si>
-  <si>
-    <t>Accounting</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -158,7 +122,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="#,##0.000\ [$₫-42A];\-#,##0.000\ [$₫-42A]"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -297,25 +261,25 @@
     <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -601,7 +565,7 @@
   <dimension ref="A1:N480"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -624,37 +588,37 @@
   <sheetData>
     <row r="1" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B1" s="14" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:14" s="12" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>0</v>
@@ -666,34 +630,34 @@
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="N2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
@@ -8360,19 +8324,7 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{146FA466-9E26-48A9-949B-0252AB269825}">
-          <x14:formula1>
-            <xm:f>List!$E$3:$E$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>F3:F1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
-          <x14:formula1>
-            <xm:f>List!$B$3:$B$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>D3:D480</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DDD68461-6E17-4B10-8E17-BC491BAA84E0}">
           <x14:formula1>
             <xm:f>List!$B$16:$B$19</xm:f>
@@ -8390,7 +8342,7 @@
   <dimension ref="A1:AC21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8407,17 +8359,17 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="10" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
@@ -8447,21 +8399,21 @@
         <v>4</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" s="8"/>
       <c r="D2" s="11" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="11" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -8487,18 +8439,16 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
-        <v>30</v>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1">
+        <v>1</v>
       </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -8524,18 +8474,16 @@
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="21" t="s">
-        <v>5</v>
-      </c>
+      <c r="B4" s="21"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
-        <v>25</v>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1">
+        <v>2</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -8561,18 +8509,16 @@
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="21" t="s">
-        <v>32</v>
-      </c>
+      <c r="B5" s="21"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="1" t="s">
-        <v>26</v>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1">
+        <v>3</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -8598,18 +8544,16 @@
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="21" t="s">
-        <v>33</v>
-      </c>
+      <c r="B6" s="21"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
-        <v>27</v>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1">
+        <v>4</v>
       </c>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -8635,14 +8579,10 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="21" t="s">
-        <v>6</v>
-      </c>
+      <c r="B7" s="21"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -8670,14 +8610,10 @@
     </row>
     <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="21" t="s">
-        <v>34</v>
-      </c>
+      <c r="B8" s="21"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>

</xml_diff>

<commit_message>
[feature] fill expense code list in file excel
</commit_message>
<xml_diff>
--- a/src/main/resources/fileTemplate/Financial Planning_v1.0.xlsx
+++ b/src/main/resources/fileTemplate/Financial Planning_v1.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\IdeaProjects\fin-planning-backend\src\main\resources\fileTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A480880E-62F5-4C8F-8ED9-A8CC252A20C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A397D280-0CD0-4791-B72C-A603120EC5B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Expense" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>DATE</t>
   </si>
@@ -100,19 +100,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>New</t>
-  </si>
-  <si>
-    <t>Waiting for approval</t>
-  </si>
-  <si>
-    <t>Approved</t>
-  </si>
-  <si>
-    <t>Denied</t>
+    <t>Code</t>
   </si>
 </sst>
 </file>
@@ -564,8 +552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N480"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8341,8 +8329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AC21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8444,12 +8432,8 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>25</v>
-      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
@@ -8479,12 +8463,8 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="1">
-        <v>2</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
@@ -8514,12 +8494,8 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1">
-        <v>3</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -8549,12 +8525,8 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="1">
-        <v>4</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>28</v>
-      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>

</xml_diff>

<commit_message>
remove schedule service, add constrain for create plan, add constraint for delete term
</commit_message>
<xml_diff>
--- a/src/main/resources/fileTemplate/Financial Planning_v1.0.xlsx
+++ b/src/main/resources/fileTemplate/Financial Planning_v1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\IdeaProjects\fin-planning-backend\src\main\resources\fileTemplate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8079E0-B3F3-4DCE-B4D4-99D3FC4734C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1617A7E5-777E-4175-9906-ECE262C3CD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>DATE</t>
   </si>
@@ -575,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P480"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -615,7 +615,9 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="K1" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="L1" s="1" t="s">
         <v>13</v>
       </c>
@@ -9284,7 +9286,7 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="decimal" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input invalid" error="Total should be greater than 0" sqref="J1:K1 J481:J1048576 K481:K1048576" xr:uid="{8A9EF7FA-9A89-4744-A79A-82C08E532854}">
+    <dataValidation type="decimal" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Input invalid" error="Total should be greater than 0" sqref="J481:K1048576 J1" xr:uid="{8A9EF7FA-9A89-4744-A79A-82C08E532854}">
       <formula1>0</formula1>
     </dataValidation>
     <dataValidation type="decimal" errorStyle="warning" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Unit price should be greater than 0" sqref="H1 H481:H1048576" xr:uid="{D2F3A8F6-0EF1-4262-9F0A-FBFD5E6E6FAD}">

</xml_diff>